<commit_message>
action:Thu Dec  8 05:51:33 UTC 2022
</commit_message>
<xml_diff>
--- a/jsl_20221208.xlsx
+++ b/jsl_20221208.xlsx
@@ -741,67 +741,67 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>128022</t>
+          <t>128069</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>众信转债</t>
+          <t>华森转债</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>zxzz</t>
+          <t>hszz</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>157.905</v>
+        <v>134.923</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.11</v>
+        <v>0.59</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>002707</t>
+          <t>002907</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>众信旅游</t>
+          <t>华森制药</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>zxly</t>
+          <t>hszy</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>9.43</v>
+        <v>24.41</v>
       </c>
       <c r="K2" t="n">
-        <v>0.96</v>
+        <v>1.08</v>
       </c>
       <c r="L2" t="n">
-        <v>26.19</v>
+        <v>7.42</v>
       </c>
       <c r="M2" t="n">
-        <v>5.95</v>
+        <v>17.97</v>
       </c>
       <c r="N2" t="n">
-        <v>158.49</v>
+        <v>135.84</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.37</v>
+        <v>-0.68</v>
       </c>
       <c r="Q2" t="n">
-        <v>157.54</v>
+        <v>134.24</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>461004</t>
+          <t>370201</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -816,7 +816,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>2017-12-28</t>
+          <t>2019-07-11</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
@@ -837,18 +837,18 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>AA-</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="n">
-        <v>4.17</v>
+        <v>12.58</v>
       </c>
       <c r="AC2" t="n">
-        <v>7.74</v>
+        <v>23.36</v>
       </c>
       <c r="AD2" t="n">
-        <v>2.6</v>
+        <v>1.9</v>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
@@ -857,21 +857,21 @@
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>23-12-01</t>
+          <t>25-06-24</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr"/>
       <c r="AH2" t="n">
-        <v>1.82</v>
+        <v>1.305</v>
       </c>
       <c r="AI2" t="n">
-        <v>192617.85</v>
+        <v>62768.72</v>
       </c>
       <c r="AJ2" t="n">
-        <v>75561.23</v>
+        <v>23365.79</v>
       </c>
       <c r="AK2" t="n">
-        <v>665.6900000000001</v>
+        <v>360.76</v>
       </c>
       <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="inlineStr"/>
@@ -880,9 +880,9 @@
       </c>
       <c r="AO2" t="inlineStr">
         <is>
-          <t>最后交易日：2022年12月15日
-最后转股日：2022年12月20日
-赎回价：100.10元/张</t>
+          <t>最后交易日：2022年12月12日
+最后转股日：2022年12月15日
+赎回价：100.72元/张</t>
         </is>
       </c>
       <c r="AP2" t="inlineStr">
@@ -892,7 +892,7 @@
       </c>
       <c r="AQ2" t="inlineStr">
         <is>
-          <t>13:37:21</t>
+          <t>13:51:00</t>
         </is>
       </c>
       <c r="AR2" t="inlineStr">
@@ -900,11 +900,7 @@
           <t>00</t>
         </is>
       </c>
-      <c r="AS2" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="inlineStr">
         <is>
           <t>Y</t>
@@ -916,31 +912,25 @@
         </is>
       </c>
       <c r="AV2" t="n">
-        <v>2</v>
-      </c>
-      <c r="AW2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0</v>
       </c>
       <c r="AX2" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="AY2" t="inlineStr">
-        <is>
-          <t>转股价下修2次，成功下修2次</t>
-        </is>
-      </c>
+      <c r="AY2" t="inlineStr"/>
       <c r="AZ2" t="inlineStr">
         <is>
-          <t>2018-06-07 开始转股</t>
+          <t>2019-12-30 开始转股</t>
         </is>
       </c>
       <c r="BA2" t="inlineStr">
         <is>
-          <t>强赎登记日2022-12-15，赎回价格100.100元，如不考虑强赎纯债价值为89.55元，计算使用1.0年期 评级为BBB 债参考YTM：18.3716</t>
+          <t>强赎登记日2022-12-12，赎回价格100.720元，如不考虑强赎纯债价值为101.78元，计算使用2.6年期 评级为AA- 债参考YTM：6.1933</t>
         </is>
       </c>
       <c r="BB2" t="inlineStr">
@@ -949,26 +939,26 @@
         </is>
       </c>
       <c r="BC2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="BD2" t="inlineStr">
         <is>
-          <t>全价：157.905 最后更新：13:37:21</t>
+          <t>全价：134.923 最后更新：13:51:00</t>
         </is>
       </c>
       <c r="BE2" t="inlineStr">
         <is>
-          <t>2022-12-15</t>
+          <t>2022-12-12</t>
         </is>
       </c>
       <c r="BF2" t="inlineStr">
         <is>
-          <t>100.100</t>
+          <t>100.720</t>
         </is>
       </c>
       <c r="BG2" t="inlineStr">
         <is>
-          <t>如不考虑强赎期权价值为70.02元</t>
+          <t>如不考虑强赎期权价值为74.14元</t>
         </is>
       </c>
       <c r="BH2" t="inlineStr"/>
@@ -998,10 +988,10 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>135.87</v>
+        <v>135.61</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.31</v>
+        <v>-1.5</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -1019,28 +1009,28 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>72.98</v>
+        <v>72.87</v>
       </c>
       <c r="K3" t="n">
-        <v>-1.37</v>
+        <v>-1.51</v>
       </c>
       <c r="L3" t="n">
-        <v>5.11</v>
+        <v>5.1</v>
       </c>
       <c r="M3" t="n">
         <v>53.59</v>
       </c>
       <c r="N3" t="n">
-        <v>136.18</v>
+        <v>135.98</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.23</v>
+        <v>-0.27</v>
       </c>
       <c r="Q3" t="n">
-        <v>135.64</v>
+        <v>135.34</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
@@ -1108,13 +1098,13 @@
         <v>2.469</v>
       </c>
       <c r="AI3" t="n">
-        <v>12733.71</v>
+        <v>13054.25</v>
       </c>
       <c r="AJ3" t="n">
-        <v>19474.98</v>
+        <v>20622.34</v>
       </c>
       <c r="AK3" t="n">
-        <v>37.74</v>
+        <v>38.7</v>
       </c>
       <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="inlineStr"/>
@@ -1135,7 +1125,7 @@
       </c>
       <c r="AQ3" t="inlineStr">
         <is>
-          <t>13:37:21</t>
+          <t>13:50:57</t>
         </is>
       </c>
       <c r="AR3" t="inlineStr">
@@ -1190,7 +1180,7 @@
       </c>
       <c r="BD3" t="inlineStr">
         <is>
-          <t>全价：135.870 最后更新：13:37:21</t>
+          <t>全价：135.610 最后更新：13:50:57</t>
         </is>
       </c>
       <c r="BE3" t="inlineStr">
@@ -1205,7 +1195,7 @@
       </c>
       <c r="BG3" t="inlineStr">
         <is>
-          <t>如不考虑强赎期权价值为82.74元</t>
+          <t>如不考虑强赎期权价值为82.52元</t>
         </is>
       </c>
       <c r="BH3" t="inlineStr"/>
@@ -1221,67 +1211,67 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>128069</t>
+          <t>128022</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>华森转债</t>
+          <t>众信转债</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>hszz</t>
+          <t>zxzz</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>132.87</v>
+        <v>158.23</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.9399999999999999</v>
+        <v>-0.91</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>002907</t>
+          <t>002707</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>华森制药</t>
+          <t>众信旅游</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>hszy</t>
+          <t>zxly</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>23.92</v>
+        <v>9.44</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.95</v>
+        <v>1.07</v>
       </c>
       <c r="L4" t="n">
-        <v>7.28</v>
+        <v>26.22</v>
       </c>
       <c r="M4" t="n">
-        <v>17.97</v>
+        <v>5.95</v>
       </c>
       <c r="N4" t="n">
-        <v>133.11</v>
+        <v>158.66</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.18</v>
+        <v>-0.27</v>
       </c>
       <c r="Q4" t="n">
-        <v>132.69</v>
+        <v>157.96</v>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>370201</t>
+          <t>461004</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -1296,7 +1286,7 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>2019-07-11</t>
+          <t>2017-12-28</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
@@ -1317,18 +1307,18 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>AA-</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="n">
-        <v>12.58</v>
+        <v>4.17</v>
       </c>
       <c r="AC4" t="n">
-        <v>23.36</v>
+        <v>7.74</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.9</v>
+        <v>2.6</v>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
@@ -1337,21 +1327,21 @@
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>25-06-24</t>
+          <t>23-12-01</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="n">
-        <v>1.305</v>
+        <v>1.82</v>
       </c>
       <c r="AI4" t="n">
-        <v>49042.43</v>
+        <v>199438.51</v>
       </c>
       <c r="AJ4" t="n">
-        <v>16790.41</v>
+        <v>78333.42</v>
       </c>
       <c r="AK4" t="n">
-        <v>282.56</v>
+        <v>689.4299999999999</v>
       </c>
       <c r="AL4" t="inlineStr"/>
       <c r="AM4" t="inlineStr"/>
@@ -1360,9 +1350,9 @@
       </c>
       <c r="AO4" t="inlineStr">
         <is>
-          <t>最后交易日：2022年12月12日
-最后转股日：2022年12月15日
-赎回价：100.72元/张</t>
+          <t>最后交易日：2022年12月15日
+最后转股日：2022年12月20日
+赎回价：100.10元/张</t>
         </is>
       </c>
       <c r="AP4" t="inlineStr">
@@ -1372,7 +1362,7 @@
       </c>
       <c r="AQ4" t="inlineStr">
         <is>
-          <t>13:37:21</t>
+          <t>13:51:00</t>
         </is>
       </c>
       <c r="AR4" t="inlineStr">
@@ -1380,7 +1370,11 @@
           <t>00</t>
         </is>
       </c>
-      <c r="AS4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="AT4" t="inlineStr">
         <is>
           <t>Y</t>
@@ -1392,25 +1386,31 @@
         </is>
       </c>
       <c r="AV4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW4" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="AX4" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="AY4" t="inlineStr"/>
+      <c r="AY4" t="inlineStr">
+        <is>
+          <t>转股价下修2次，成功下修2次</t>
+        </is>
+      </c>
       <c r="AZ4" t="inlineStr">
         <is>
-          <t>2019-12-30 开始转股</t>
+          <t>2018-06-07 开始转股</t>
         </is>
       </c>
       <c r="BA4" t="inlineStr">
         <is>
-          <t>强赎登记日2022-12-12，赎回价格100.720元，如不考虑强赎纯债价值为101.78元，计算使用2.6年期 评级为AA- 债参考YTM：6.1933</t>
+          <t>强赎登记日2022-12-15，赎回价格100.100元，如不考虑强赎纯债价值为89.55元，计算使用1.0年期 评级为BBB 债参考YTM：18.3716</t>
         </is>
       </c>
       <c r="BB4" t="inlineStr">
@@ -1419,26 +1419,26 @@
         </is>
       </c>
       <c r="BC4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BD4" t="inlineStr">
         <is>
-          <t>全价：132.870 最后更新：13:37:21</t>
+          <t>全价：158.230 最后更新：13:51:00</t>
         </is>
       </c>
       <c r="BE4" t="inlineStr">
         <is>
-          <t>2022-12-12</t>
+          <t>2022-12-15</t>
         </is>
       </c>
       <c r="BF4" t="inlineStr">
         <is>
-          <t>100.720</t>
+          <t>100.100</t>
         </is>
       </c>
       <c r="BG4" t="inlineStr">
         <is>
-          <t>如不考虑强赎期权价值为72.10元</t>
+          <t>如不考虑强赎期权价值为70.31元</t>
         </is>
       </c>
       <c r="BH4" t="inlineStr"/>
@@ -1454,72 +1454,72 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>110061</t>
+          <t>128029</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>川投转债</t>
+          <t>太阳转债</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ctzz</t>
+          <t>tyzz</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>132.061</v>
+        <v>133.209</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.6</v>
+        <v>-0.88</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>600674</t>
+          <t>002078</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>川投能源</t>
+          <t>太阳纸业</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>ctny</t>
+          <t>tyzy</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>11.64</v>
+        <v>11.01</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.51</v>
+        <v>-0.63</v>
       </c>
       <c r="L5" t="n">
-        <v>1.59</v>
+        <v>1.37</v>
       </c>
       <c r="M5" t="n">
-        <v>8.800000000000001</v>
+        <v>8.25</v>
       </c>
       <c r="N5" t="n">
-        <v>132.27</v>
+        <v>133.45</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.16</v>
+        <v>-0.18</v>
       </c>
       <c r="Q5" t="n">
-        <v>131.9</v>
+        <v>133.03</v>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>410102</t>
+          <t>360102</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>shmb</t>
+          <t>szmb</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>2019-12-02</t>
+          <t>2018-01-16</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
@@ -1550,18 +1550,18 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>AAA</t>
+          <t>AA+</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="n">
-        <v>6.16</v>
+        <v>5.78</v>
       </c>
       <c r="AC5" t="n">
-        <v>11.44</v>
+        <v>10.73</v>
       </c>
       <c r="AD5" t="n">
-        <v>6.8</v>
+        <v>1.2</v>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
@@ -1570,36 +1570,44 @@
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>25-11-10</t>
+          <t>22-12-22</t>
         </is>
       </c>
       <c r="AG5" t="n">
-        <v>2.926</v>
+        <v>0.038</v>
       </c>
       <c r="AH5" t="n">
-        <v>34.983</v>
+        <v>3.38</v>
       </c>
       <c r="AI5" t="n">
-        <v>3567.49</v>
+        <v>3404.96</v>
       </c>
       <c r="AJ5" t="n">
-        <v>9250.959999999999</v>
+        <v>8796.34</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.77</v>
+        <v>7.57</v>
       </c>
       <c r="AL5" t="n">
-        <v>-6.35</v>
+        <v>-537.52</v>
       </c>
       <c r="AM5" t="inlineStr"/>
       <c r="AN5" t="n">
         <v>0</v>
       </c>
-      <c r="AO5" t="inlineStr"/>
-      <c r="AP5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>2022年1月1日公告：本次不提前赎回，至存续期结束前（即2022年12月22日前）均不行使提前赎回权利</t>
+        </is>
+      </c>
+      <c r="AP5" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
       <c r="AQ5" t="inlineStr">
         <is>
-          <t>13:37:21</t>
+          <t>13:50:51</t>
         </is>
       </c>
       <c r="AR5" t="inlineStr">
@@ -1636,12 +1644,12 @@
       <c r="AY5" t="inlineStr"/>
       <c r="AZ5" t="inlineStr">
         <is>
-          <t>2020-05-15 开始转股</t>
+          <t>2018-06-28 开始转股</t>
         </is>
       </c>
       <c r="BA5" t="inlineStr">
         <is>
-          <t>计算使用3.0年期 评级为AAA 债参考YTM：3.3259</t>
+          <t>计算使用0.1年期 评级为AA+ 债参考YTM：2.4981</t>
         </is>
       </c>
       <c r="BB5" t="inlineStr">
@@ -1650,11 +1658,11 @@
         </is>
       </c>
       <c r="BC5" t="n">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="BD5" t="inlineStr">
         <is>
-          <t>全价：132.061 最后更新：13:37:21</t>
+          <t>全价：133.209 最后更新：13:50:51</t>
         </is>
       </c>
       <c r="BE5" t="inlineStr"/>
@@ -1673,72 +1681,72 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>128029</t>
+          <t>110061</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>太阳转债</t>
+          <t>川投转债</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>tyzz</t>
+          <t>ctzz</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>133.53</v>
+        <v>131.96</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.64</v>
+        <v>-0.68</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>002078</t>
+          <t>600674</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>太阳纸业</t>
+          <t>川投能源</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>tyzy</t>
+          <t>ctny</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>11.02</v>
+        <v>11.62</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.54</v>
+        <v>-0.68</v>
       </c>
       <c r="L6" t="n">
-        <v>1.37</v>
+        <v>1.59</v>
       </c>
       <c r="M6" t="n">
-        <v>8.25</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="N6" t="n">
-        <v>133.58</v>
+        <v>132.05</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.04</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="Q6" t="n">
-        <v>133.49</v>
+        <v>131.89</v>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>360102</t>
+          <t>410102</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>szmb</t>
+          <t>shmb</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -1748,7 +1756,7 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>2018-01-16</t>
+          <t>2019-12-02</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
@@ -1769,18 +1777,18 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>AA+</t>
+          <t>AAA</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="n">
-        <v>5.78</v>
+        <v>6.16</v>
       </c>
       <c r="AC6" t="n">
-        <v>10.73</v>
+        <v>11.44</v>
       </c>
       <c r="AD6" t="n">
-        <v>1.2</v>
+        <v>6.8</v>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
@@ -1789,44 +1797,36 @@
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>22-12-22</t>
+          <t>25-11-10</t>
         </is>
       </c>
       <c r="AG6" t="n">
-        <v>0.038</v>
+        <v>2.926</v>
       </c>
       <c r="AH6" t="n">
-        <v>3.38</v>
+        <v>34.983</v>
       </c>
       <c r="AI6" t="n">
-        <v>3361.36</v>
+        <v>4115.3</v>
       </c>
       <c r="AJ6" t="n">
-        <v>8385.709999999999</v>
+        <v>10899.75</v>
       </c>
       <c r="AK6" t="n">
-        <v>7.47</v>
+        <v>0.89</v>
       </c>
       <c r="AL6" t="n">
-        <v>-542.5599999999999</v>
+        <v>-6.32</v>
       </c>
       <c r="AM6" t="inlineStr"/>
       <c r="AN6" t="n">
         <v>0</v>
       </c>
-      <c r="AO6" t="inlineStr">
-        <is>
-          <t>2022年1月1日公告：本次不提前赎回，至存续期结束前（即2022年12月22日前）均不行使提前赎回权利</t>
-        </is>
-      </c>
-      <c r="AP6" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="inlineStr"/>
       <c r="AQ6" t="inlineStr">
         <is>
-          <t>13:37:21</t>
+          <t>13:50:57</t>
         </is>
       </c>
       <c r="AR6" t="inlineStr">
@@ -1863,12 +1863,12 @@
       <c r="AY6" t="inlineStr"/>
       <c r="AZ6" t="inlineStr">
         <is>
-          <t>2018-06-28 开始转股</t>
+          <t>2020-05-15 开始转股</t>
         </is>
       </c>
       <c r="BA6" t="inlineStr">
         <is>
-          <t>计算使用0.1年期 评级为AA+ 债参考YTM：2.4981</t>
+          <t>计算使用3.0年期 评级为AAA 债参考YTM：3.3259</t>
         </is>
       </c>
       <c r="BB6" t="inlineStr">
@@ -1877,11 +1877,11 @@
         </is>
       </c>
       <c r="BC6" t="n">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="BD6" t="inlineStr">
         <is>
-          <t>全价：133.530 最后更新：13:37:21</t>
+          <t>全价：131.960 最后更新：13:50:57</t>
         </is>
       </c>
       <c r="BE6" t="inlineStr"/>
@@ -1914,10 +1914,10 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>138.618</v>
+        <v>137.101</v>
       </c>
       <c r="F7" t="n">
-        <v>0.09</v>
+        <v>-1.01</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -1935,28 +1935,28 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>24.23</v>
+        <v>24.02</v>
       </c>
       <c r="K7" t="n">
-        <v>0.12</v>
+        <v>-0.74</v>
       </c>
       <c r="L7" t="n">
-        <v>3.66</v>
+        <v>3.63</v>
       </c>
       <c r="M7" t="n">
         <v>17.51</v>
       </c>
       <c r="N7" t="n">
-        <v>138.38</v>
+        <v>137.18</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>0.17</v>
+        <v>-0.06</v>
       </c>
       <c r="Q7" t="n">
-        <v>138.79</v>
+        <v>137.04</v>
       </c>
       <c r="R7" t="inlineStr">
         <is>
@@ -2007,7 +2007,7 @@
         <v>22.76</v>
       </c>
       <c r="AD7" t="n">
-        <v>11.6</v>
+        <v>11.8</v>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
@@ -2026,16 +2026,16 @@
         <v>8.784000000000001</v>
       </c>
       <c r="AI7" t="n">
-        <v>28868.2</v>
+        <v>29692.76</v>
       </c>
       <c r="AJ7" t="n">
-        <v>16201.5</v>
+        <v>17100.01</v>
       </c>
       <c r="AK7" t="n">
-        <v>23.62</v>
+        <v>24.3</v>
       </c>
       <c r="AL7" t="n">
-        <v>-4.97</v>
+        <v>-4.75</v>
       </c>
       <c r="AM7" t="inlineStr"/>
       <c r="AN7" t="n">
@@ -2045,7 +2045,7 @@
       <c r="AP7" t="inlineStr"/>
       <c r="AQ7" t="inlineStr">
         <is>
-          <t>13:37:21</t>
+          <t>13:51:00</t>
         </is>
       </c>
       <c r="AR7" t="inlineStr">
@@ -2100,7 +2100,7 @@
       </c>
       <c r="BD7" t="inlineStr">
         <is>
-          <t>全价：138.618 最后更新：13:37:21</t>
+          <t>全价：137.101 最后更新：13:51:00</t>
         </is>
       </c>
       <c r="BE7" t="inlineStr"/>
@@ -2133,10 +2133,10 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>126.987</v>
+        <v>126.821</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6</v>
+        <v>0.47</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>7.49</v>
+        <v>7.5</v>
       </c>
       <c r="K8" t="n">
-        <v>0.9399999999999999</v>
+        <v>1.08</v>
       </c>
       <c r="L8" t="n">
         <v>0.54</v>
@@ -2166,16 +2166,16 @@
         <v>5.97</v>
       </c>
       <c r="N8" t="n">
-        <v>125.46</v>
+        <v>125.63</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>1.22</v>
+        <v>0.95</v>
       </c>
       <c r="Q8" t="n">
-        <v>128.21</v>
+        <v>127.77</v>
       </c>
       <c r="R8" t="inlineStr">
         <is>
@@ -2243,16 +2243,16 @@
         <v>199.992</v>
       </c>
       <c r="AI8" t="n">
-        <v>18709.4</v>
+        <v>19472.32</v>
       </c>
       <c r="AJ8" t="n">
-        <v>40764.04</v>
+        <v>41936.97</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.74</v>
+        <v>0.77</v>
       </c>
       <c r="AL8" t="n">
-        <v>-3.74</v>
+        <v>-3.68</v>
       </c>
       <c r="AM8" t="inlineStr"/>
       <c r="AN8" t="n">
@@ -2262,7 +2262,7 @@
       <c r="AP8" t="inlineStr"/>
       <c r="AQ8" t="inlineStr">
         <is>
-          <t>13:37:21</t>
+          <t>13:50:58</t>
         </is>
       </c>
       <c r="AR8" t="inlineStr">
@@ -2317,7 +2317,7 @@
       </c>
       <c r="BD8" t="inlineStr">
         <is>
-          <t>全价：126.987 最后更新：13:37:21</t>
+          <t>全价：126.821 最后更新：13:50:58</t>
         </is>
       </c>
       <c r="BE8" t="inlineStr"/>
@@ -2336,67 +2336,67 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>128081</t>
+          <t>128087</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>海亮转债</t>
+          <t>孚日转债</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>hlzz</t>
+          <t>frzz</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>129.119</v>
+        <v>131.352</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.29</v>
+        <v>0.27</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>002203</t>
+          <t>002083</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>海亮股份</t>
+          <t>孚日股份</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>hlgf</t>
+          <t>frgf</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>12.25</v>
+        <v>5.4</v>
       </c>
       <c r="K9" t="n">
-        <v>0.16</v>
+        <v>1.12</v>
       </c>
       <c r="L9" t="n">
-        <v>1.98</v>
+        <v>1.18</v>
       </c>
       <c r="M9" t="n">
-        <v>9.619999999999999</v>
+        <v>4.16</v>
       </c>
       <c r="N9" t="n">
-        <v>127.34</v>
+        <v>129.81</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>1.4</v>
+        <v>1.19</v>
       </c>
       <c r="Q9" t="n">
-        <v>130.52</v>
+        <v>132.54</v>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>240302</t>
+          <t>350102</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>2019-12-16</t>
+          <t>2020-01-16</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
@@ -2432,18 +2432,18 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>AA-</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="n">
-        <v>6.73</v>
+        <v>2.91</v>
       </c>
       <c r="AC9" t="n">
-        <v>12.51</v>
+        <v>5.41</v>
       </c>
       <c r="AD9" t="n">
-        <v>12.4</v>
+        <v>14.8</v>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
@@ -2452,26 +2452,26 @@
       </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>25-11-21</t>
+          <t>25-12-17</t>
         </is>
       </c>
       <c r="AG9" t="n">
-        <v>2.956</v>
+        <v>3.027</v>
       </c>
       <c r="AH9" t="n">
-        <v>29.236</v>
+        <v>6.46</v>
       </c>
       <c r="AI9" t="n">
-        <v>8588.35</v>
+        <v>38019.11</v>
       </c>
       <c r="AJ9" t="n">
-        <v>3497.99</v>
+        <v>25354.6</v>
       </c>
       <c r="AK9" t="n">
-        <v>2.28</v>
+        <v>43.9</v>
       </c>
       <c r="AL9" t="n">
-        <v>-4.38</v>
+        <v>-5.15</v>
       </c>
       <c r="AM9" t="inlineStr"/>
       <c r="AN9" t="n">
@@ -2481,7 +2481,7 @@
       <c r="AP9" t="inlineStr"/>
       <c r="AQ9" t="inlineStr">
         <is>
-          <t>13:37:21</t>
+          <t>13:51:00</t>
         </is>
       </c>
       <c r="AR9" t="inlineStr">
@@ -2489,11 +2489,7 @@
           <t>00</t>
         </is>
       </c>
-      <c r="AS9" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="AS9" t="inlineStr"/>
       <c r="AT9" t="inlineStr">
         <is>
           <t>Y</t>
@@ -2505,25 +2501,31 @@
         </is>
       </c>
       <c r="AV9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW9" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AW9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="AX9" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="AY9" t="inlineStr"/>
+      <c r="AY9" t="inlineStr">
+        <is>
+          <t>转股价下修1次，成功下修1次</t>
+        </is>
+      </c>
       <c r="AZ9" t="inlineStr">
         <is>
-          <t>2020-05-27 开始转股</t>
+          <t>2020-06-23 开始转股</t>
         </is>
       </c>
       <c r="BA9" t="inlineStr">
         <is>
-          <t>计算使用3.0年期 评级为AA 债参考YTM：3.8584</t>
+          <t>计算使用3.1年期 评级为AA- 债参考YTM：6.2670</t>
         </is>
       </c>
       <c r="BB9" t="inlineStr">
@@ -2532,11 +2534,11 @@
         </is>
       </c>
       <c r="BC9" t="n">
-        <v>31.5</v>
+        <v>6.5</v>
       </c>
       <c r="BD9" t="inlineStr">
         <is>
-          <t>全价：129.119 最后更新：13:37:21</t>
+          <t>全价：131.352 最后更新：13:51:00</t>
         </is>
       </c>
       <c r="BE9" t="inlineStr"/>
@@ -2555,67 +2557,67 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>128087</t>
+          <t>128081</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>孚日转债</t>
+          <t>海亮转债</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>frzz</t>
+          <t>hlzz</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>131.24</v>
+        <v>128.783</v>
       </c>
       <c r="F10" t="n">
-        <v>0.18</v>
+        <v>-0.55</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>002083</t>
+          <t>002203</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>孚日股份</t>
+          <t>海亮股份</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>frgf</t>
+          <t>hlgf</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>5.37</v>
+        <v>12.22</v>
       </c>
       <c r="K10" t="n">
-        <v>0.5600000000000001</v>
+        <v>-0.08</v>
       </c>
       <c r="L10" t="n">
-        <v>1.17</v>
+        <v>1.98</v>
       </c>
       <c r="M10" t="n">
-        <v>4.16</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="N10" t="n">
-        <v>129.09</v>
+        <v>127.03</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>1.67</v>
+        <v>1.38</v>
       </c>
       <c r="Q10" t="n">
-        <v>132.91</v>
+        <v>130.16</v>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>350102</t>
+          <t>240302</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -2630,7 +2632,7 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>2020-01-16</t>
+          <t>2019-12-16</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
@@ -2651,18 +2653,18 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>AA-</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="n">
-        <v>2.91</v>
+        <v>6.73</v>
       </c>
       <c r="AC10" t="n">
-        <v>5.41</v>
+        <v>12.51</v>
       </c>
       <c r="AD10" t="n">
-        <v>14.9</v>
+        <v>12.4</v>
       </c>
       <c r="AE10" t="inlineStr">
         <is>
@@ -2671,26 +2673,26 @@
       </c>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>25-12-17</t>
+          <t>25-11-21</t>
         </is>
       </c>
       <c r="AG10" t="n">
-        <v>3.027</v>
+        <v>2.956</v>
       </c>
       <c r="AH10" t="n">
-        <v>6.46</v>
+        <v>29.236</v>
       </c>
       <c r="AI10" t="n">
-        <v>37444.76</v>
+        <v>8861.110000000001</v>
       </c>
       <c r="AJ10" t="n">
-        <v>24810.52</v>
+        <v>5105.37</v>
       </c>
       <c r="AK10" t="n">
-        <v>43.22</v>
+        <v>2.35</v>
       </c>
       <c r="AL10" t="n">
-        <v>-5.13</v>
+        <v>-4.3</v>
       </c>
       <c r="AM10" t="inlineStr"/>
       <c r="AN10" t="n">
@@ -2700,7 +2702,7 @@
       <c r="AP10" t="inlineStr"/>
       <c r="AQ10" t="inlineStr">
         <is>
-          <t>13:37:18</t>
+          <t>13:51:00</t>
         </is>
       </c>
       <c r="AR10" t="inlineStr">
@@ -2708,7 +2710,11 @@
           <t>00</t>
         </is>
       </c>
-      <c r="AS10" t="inlineStr"/>
+      <c r="AS10" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="AT10" t="inlineStr">
         <is>
           <t>Y</t>
@@ -2720,31 +2726,25 @@
         </is>
       </c>
       <c r="AV10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>0</v>
       </c>
       <c r="AX10" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="AY10" t="inlineStr">
-        <is>
-          <t>转股价下修1次，成功下修1次</t>
-        </is>
-      </c>
+      <c r="AY10" t="inlineStr"/>
       <c r="AZ10" t="inlineStr">
         <is>
-          <t>2020-06-23 开始转股</t>
+          <t>2020-05-27 开始转股</t>
         </is>
       </c>
       <c r="BA10" t="inlineStr">
         <is>
-          <t>计算使用3.1年期 评级为AA- 债参考YTM：6.2670</t>
+          <t>计算使用3.0年期 评级为AA 债参考YTM：3.8584</t>
         </is>
       </c>
       <c r="BB10" t="inlineStr">
@@ -2753,11 +2753,11 @@
         </is>
       </c>
       <c r="BC10" t="n">
-        <v>6.5</v>
+        <v>31.5</v>
       </c>
       <c r="BD10" t="inlineStr">
         <is>
-          <t>全价：131.240 最后更新：13:37:18</t>
+          <t>全价：128.783 最后更新：13:51:00</t>
         </is>
       </c>
       <c r="BE10" t="inlineStr"/>
@@ -2790,10 +2790,10 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>226.862</v>
+        <v>226.88</v>
       </c>
       <c r="F11" t="n">
-        <v>4.32</v>
+        <v>4.33</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2811,10 +2811,10 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>27.84</v>
+        <v>27.9</v>
       </c>
       <c r="K11" t="n">
-        <v>1.53</v>
+        <v>1.75</v>
       </c>
       <c r="L11" t="n">
         <v>2.8</v>
@@ -2823,16 +2823,16 @@
         <v>12.55</v>
       </c>
       <c r="N11" t="n">
-        <v>221.83</v>
+        <v>222.31</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>2.27</v>
+        <v>2.06</v>
       </c>
       <c r="Q11" t="n">
-        <v>229.13</v>
+        <v>228.94</v>
       </c>
       <c r="R11" t="inlineStr">
         <is>
@@ -2902,16 +2902,16 @@
         <v>8.472</v>
       </c>
       <c r="AI11" t="n">
-        <v>57749.21</v>
+        <v>65734.77</v>
       </c>
       <c r="AJ11" t="n">
-        <v>8582.200000000001</v>
+        <v>9468.42</v>
       </c>
       <c r="AK11" t="n">
-        <v>30.63</v>
+        <v>34.78</v>
       </c>
       <c r="AL11" t="n">
-        <v>-15.38</v>
+        <v>-15.39</v>
       </c>
       <c r="AM11" t="inlineStr"/>
       <c r="AN11" t="n">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="AQ11" t="inlineStr">
         <is>
-          <t>13:37:21</t>
+          <t>13:51:01</t>
         </is>
       </c>
       <c r="AR11" t="inlineStr">
@@ -2984,7 +2984,7 @@
       </c>
       <c r="BD11" t="inlineStr">
         <is>
-          <t>全价：226.862 最后更新：13:37:21</t>
+          <t>全价：226.880 最后更新：13:51:01</t>
         </is>
       </c>
       <c r="BE11" t="inlineStr"/>

</xml_diff>